<commit_message>
Suppression de la contrainte "contained" obligatoire pour les champs subject (#40)
* delete constr-cdr-maj rule, rm subject contained, use intendedRecipient and rm PDSm custom extension

* rm useles min 0 card

* remove Patient cardinality 0..0 from bundle

* remove useless slicenames

* remove contained subject from FolderComprehensive

* fix typo eed9b63acfd46483947cc17c57ed5c35a9072d72
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-pdsm-comprehensive-provide-document-bundle.xlsx
+++ b/ig/main/StructureDefinition-pdsm-comprehensive-provide-document-bundle.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-11T09:02:50+00:00</t>
+    <t>2023-07-21T12:08:41+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -30095,7 +30095,7 @@
         <v>36</v>
       </c>
       <c r="G248" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H248" t="s" s="2">
         <v>35</v>

</xml_diff>